<commit_message>
Extended tabular data to include primate and lagomorph references
</commit_message>
<xml_diff>
--- a/tabular/ifnl-data.xlsx
+++ b/tabular/ifnl-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11920" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="15840" yWindow="260" windowWidth="30940" windowHeight="19620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
   <si>
     <t>Camelus_bactriaus_IFNL1</t>
   </si>
@@ -76,6 +76,54 @@
   </si>
   <si>
     <t>Interferon lambda 1</t>
+  </si>
+  <si>
+    <t>Ochotona_princeps_IFNL1</t>
+  </si>
+  <si>
+    <t>Oryctolagus_cuniculus_IFNL1</t>
+  </si>
+  <si>
+    <t>Cebus_capucinus_IFNL1</t>
+  </si>
+  <si>
+    <t>Cercocebus_atys_IFNL1</t>
+  </si>
+  <si>
+    <t>Colobus_angolensis_palliatus_IFNL1</t>
+  </si>
+  <si>
+    <t>Gorilla_gorilla_IFNL1</t>
+  </si>
+  <si>
+    <t>Homo_sapiens_IFNL1</t>
+  </si>
+  <si>
+    <t>Macaca_fascicularis_IFNL1</t>
+  </si>
+  <si>
+    <t>Macaca_fuscata_IFNL1</t>
+  </si>
+  <si>
+    <t>Macaca_mulatta_IFNL1</t>
+  </si>
+  <si>
+    <t>Macaca_nemestrina_IFNL1</t>
+  </si>
+  <si>
+    <t>Mandrillus_leucophaeus_IFNL1</t>
+  </si>
+  <si>
+    <t>Pongo_abelii_IFNL1</t>
+  </si>
+  <si>
+    <t>Propithecus_coquereli_IFNL1</t>
+  </si>
+  <si>
+    <t>Saimiri_boliviensis_IFNL1</t>
+  </si>
+  <si>
+    <t>Theropithecus_gelada_IFNL1</t>
   </si>
 </sst>
 </file>
@@ -487,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:C15"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
@@ -662,6 +710,182 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated tabular data for root and internal alignment sequences
</commit_message>
<xml_diff>
--- a/tabular/ifnl-data.xlsx
+++ b/tabular/ifnl-data.xlsx
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4460,9 +4460,7 @@
       <c r="A66" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B66" s="19">
-        <v>1</v>
-      </c>
+      <c r="B66" s="19"/>
       <c r="C66" s="6" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added new sources and sequences
</commit_message>
<xml_diff>
--- a/tabular/ifnl-data.xlsx
+++ b/tabular/ifnl-data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="700" windowWidth="33880" windowHeight="25040" tabRatio="500"/>
+    <workbookView xWindow="7680" yWindow="760" windowWidth="38000" windowHeight="24840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="317">
   <si>
     <t>Locus ID</t>
   </si>
@@ -760,6 +761,216 @@
   </si>
   <si>
     <t>Aln-A1-PSI1</t>
+  </si>
+  <si>
+    <t>XM_016209155.1</t>
+  </si>
+  <si>
+    <t>LOC107534162</t>
+  </si>
+  <si>
+    <t>XM_016209154.1</t>
+  </si>
+  <si>
+    <t>LOC107534161</t>
+  </si>
+  <si>
+    <t>XM_016209156.1</t>
+  </si>
+  <si>
+    <t>LOC107534163</t>
+  </si>
+  <si>
+    <t>XM_016166771.1</t>
+  </si>
+  <si>
+    <t>LOC107521776</t>
+  </si>
+  <si>
+    <t>XM_028529978.1</t>
+  </si>
+  <si>
+    <t>Phyllostomus</t>
+  </si>
+  <si>
+    <t>discolor</t>
+  </si>
+  <si>
+    <t>LOC114511296</t>
+  </si>
+  <si>
+    <t>XM_016165226.1</t>
+  </si>
+  <si>
+    <t>LOC107520938</t>
+  </si>
+  <si>
+    <t>HQ201955.1</t>
+  </si>
+  <si>
+    <t>XM_023760578.1</t>
+  </si>
+  <si>
+    <t>lucifugus</t>
+  </si>
+  <si>
+    <t>LOC102440098</t>
+  </si>
+  <si>
+    <t>XM_006096748.3</t>
+  </si>
+  <si>
+    <t>XM_023760577.1</t>
+  </si>
+  <si>
+    <t>XM_023760554.1</t>
+  </si>
+  <si>
+    <t>LOC102438841</t>
+  </si>
+  <si>
+    <t>XM_006761471.2</t>
+  </si>
+  <si>
+    <t>davidii</t>
+  </si>
+  <si>
+    <t>LOC102774772</t>
+  </si>
+  <si>
+    <t>XM_019666264.1</t>
+  </si>
+  <si>
+    <t>LOC109395355</t>
+  </si>
+  <si>
+    <t>XM_015557658.1</t>
+  </si>
+  <si>
+    <t>LOC102768489</t>
+  </si>
+  <si>
+    <t>XM_015589199.2</t>
+  </si>
+  <si>
+    <t>LOC102889807</t>
+  </si>
+  <si>
+    <t>XM_016165227.1</t>
+  </si>
+  <si>
+    <t>LOC107520939</t>
+  </si>
+  <si>
+    <t>XM_023760555.1</t>
+  </si>
+  <si>
+    <t>LOC102439443</t>
+  </si>
+  <si>
+    <t>XM_015589198.1</t>
+  </si>
+  <si>
+    <t>LOC102889565</t>
+  </si>
+  <si>
+    <t>XM_011386751.1</t>
+  </si>
+  <si>
+    <t>vampyrus</t>
+  </si>
+  <si>
+    <t>LOC105310596</t>
+  </si>
+  <si>
+    <t>XM_008161658.2</t>
+  </si>
+  <si>
+    <t>LOC103304876</t>
+  </si>
+  <si>
+    <t>XM_024577418.1</t>
+  </si>
+  <si>
+    <t>LOC112320030</t>
+  </si>
+  <si>
+    <t>XM_024577417.1</t>
+  </si>
+  <si>
+    <t>LOC112320026</t>
+  </si>
+  <si>
+    <t>XM_005886334.2</t>
+  </si>
+  <si>
+    <t>LOC102254487</t>
+  </si>
+  <si>
+    <t>XM_005886333.2</t>
+  </si>
+  <si>
+    <t>LOC102254184</t>
+  </si>
+  <si>
+    <t>XM_005886332.2</t>
+  </si>
+  <si>
+    <t>LOC102253881</t>
+  </si>
+  <si>
+    <t>XM_014541703.1</t>
+  </si>
+  <si>
+    <t>LOC102244333</t>
+  </si>
+  <si>
+    <t>NM_001290171.1</t>
+  </si>
+  <si>
+    <t>LOC107521777</t>
+  </si>
+  <si>
+    <t>XM_028529971.1</t>
+  </si>
+  <si>
+    <t>LOC114511290</t>
+  </si>
+  <si>
+    <t>XM_028529967.1</t>
+  </si>
+  <si>
+    <t>LOC114511283</t>
+  </si>
+  <si>
+    <t>XM_028529976.1</t>
+  </si>
+  <si>
+    <t>LOC114511294</t>
+  </si>
+  <si>
+    <t>XM_028530311.1</t>
+  </si>
+  <si>
+    <t>LOC114511582</t>
+  </si>
+  <si>
+    <t>XM_024577416.1</t>
+  </si>
+  <si>
+    <t>LOC112320025</t>
+  </si>
+  <si>
+    <t>XM_019666252.1</t>
+  </si>
+  <si>
+    <t>LOC109395336</t>
+  </si>
+  <si>
+    <t>XM_028529999.1</t>
+  </si>
+  <si>
+    <t>LOC114511308</t>
   </si>
 </sst>
 </file>
@@ -772,6 +983,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -882,7 +1094,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="287">
+  <cellStyleXfs count="309">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1170,8 +1382,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1208,8 +1442,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="287">
+  <cellStyles count="309">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1353,6 +1588,17 @@
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1496,6 +1742,17 @@
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1825,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S81"/>
+  <dimension ref="A1:S121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4899,9 +5156,7 @@
         <v>175</v>
       </c>
       <c r="B77" s="15"/>
-      <c r="C77" s="11" t="s">
-        <v>182</v>
-      </c>
+      <c r="C77" s="11"/>
       <c r="D77" s="10" t="s">
         <v>164</v>
       </c>
@@ -5083,6 +5338,206 @@
       <c r="P81" s="13">
         <v>0</v>
       </c>
+    </row>
+    <row r="82" spans="1:16">
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+    </row>
+    <row r="83" spans="1:16">
+      <c r="M83"/>
+      <c r="N83"/>
+      <c r="O83"/>
+    </row>
+    <row r="84" spans="1:16">
+      <c r="M84"/>
+      <c r="N84"/>
+      <c r="O84"/>
+    </row>
+    <row r="85" spans="1:16">
+      <c r="M85"/>
+      <c r="N85"/>
+      <c r="O85"/>
+    </row>
+    <row r="86" spans="1:16">
+      <c r="M86"/>
+      <c r="N86"/>
+      <c r="O86"/>
+    </row>
+    <row r="87" spans="1:16">
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+    </row>
+    <row r="88" spans="1:16">
+      <c r="M88"/>
+      <c r="N88"/>
+      <c r="O88"/>
+    </row>
+    <row r="89" spans="1:16">
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+    </row>
+    <row r="90" spans="1:16">
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+    </row>
+    <row r="91" spans="1:16">
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
+    </row>
+    <row r="92" spans="1:16">
+      <c r="M92"/>
+      <c r="N92"/>
+      <c r="O92"/>
+    </row>
+    <row r="93" spans="1:16">
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+    </row>
+    <row r="94" spans="1:16">
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+    </row>
+    <row r="95" spans="1:16">
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+    </row>
+    <row r="96" spans="1:16">
+      <c r="M96"/>
+      <c r="N96"/>
+      <c r="O96"/>
+    </row>
+    <row r="97" spans="13:15">
+      <c r="M97"/>
+      <c r="N97"/>
+      <c r="O97"/>
+    </row>
+    <row r="98" spans="13:15">
+      <c r="M98"/>
+      <c r="N98"/>
+      <c r="O98"/>
+    </row>
+    <row r="99" spans="13:15">
+      <c r="M99"/>
+      <c r="N99"/>
+      <c r="O99"/>
+    </row>
+    <row r="100" spans="13:15">
+      <c r="M100"/>
+      <c r="N100"/>
+      <c r="O100"/>
+    </row>
+    <row r="101" spans="13:15">
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+    </row>
+    <row r="102" spans="13:15">
+      <c r="M102"/>
+      <c r="N102"/>
+      <c r="O102"/>
+    </row>
+    <row r="103" spans="13:15">
+      <c r="M103"/>
+      <c r="N103"/>
+      <c r="O103"/>
+    </row>
+    <row r="104" spans="13:15">
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+    </row>
+    <row r="105" spans="13:15">
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+    </row>
+    <row r="106" spans="13:15">
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+    </row>
+    <row r="107" spans="13:15">
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107"/>
+    </row>
+    <row r="108" spans="13:15">
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+    </row>
+    <row r="109" spans="13:15">
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+    </row>
+    <row r="110" spans="13:15">
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+    </row>
+    <row r="111" spans="13:15">
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+    </row>
+    <row r="112" spans="13:15">
+      <c r="M112"/>
+      <c r="N112"/>
+      <c r="O112"/>
+    </row>
+    <row r="113" spans="13:15">
+      <c r="M113"/>
+      <c r="N113"/>
+      <c r="O113"/>
+    </row>
+    <row r="114" spans="13:15">
+      <c r="M114"/>
+      <c r="N114"/>
+      <c r="O114"/>
+    </row>
+    <row r="115" spans="13:15">
+      <c r="M115"/>
+      <c r="N115"/>
+      <c r="O115"/>
+    </row>
+    <row r="116" spans="13:15">
+      <c r="M116"/>
+      <c r="N116"/>
+      <c r="O116"/>
+    </row>
+    <row r="117" spans="13:15">
+      <c r="M117"/>
+      <c r="N117"/>
+      <c r="O117"/>
+    </row>
+    <row r="118" spans="13:15">
+      <c r="M118"/>
+      <c r="N118"/>
+      <c r="O118"/>
+    </row>
+    <row r="119" spans="13:15">
+      <c r="M119"/>
+      <c r="N119"/>
+      <c r="O119"/>
+    </row>
+    <row r="120" spans="13:15">
+      <c r="M120"/>
+      <c r="N120"/>
+      <c r="O120"/>
+    </row>
+    <row r="121" spans="13:15">
+      <c r="M121"/>
+      <c r="N121"/>
+      <c r="O121"/>
     </row>
   </sheetData>
   <sortState ref="A2:S81">
@@ -5120,4 +5575,873 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>252</v>
+      </c>
+      <c r="H3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>260</v>
+      </c>
+      <c r="H6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>271</v>
+      </c>
+      <c r="H12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>273</v>
+      </c>
+      <c r="H13" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>275</v>
+      </c>
+      <c r="H14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>277</v>
+      </c>
+      <c r="H15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>279</v>
+      </c>
+      <c r="H16" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>281</v>
+      </c>
+      <c r="H17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>283</v>
+      </c>
+      <c r="H18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>286</v>
+      </c>
+      <c r="H19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>288</v>
+      </c>
+      <c r="H20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H21" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>292</v>
+      </c>
+      <c r="H22" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>294</v>
+      </c>
+      <c r="H23" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>296</v>
+      </c>
+      <c r="H24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>298</v>
+      </c>
+      <c r="H25" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>300</v>
+      </c>
+      <c r="H26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>302</v>
+      </c>
+      <c r="H28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>304</v>
+      </c>
+      <c r="H30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
+        <v>306</v>
+      </c>
+      <c r="H31" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>308</v>
+      </c>
+      <c r="H32" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" t="s">
+        <v>310</v>
+      </c>
+      <c r="H33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>312</v>
+      </c>
+      <c r="H34" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="s">
+        <v>314</v>
+      </c>
+      <c r="H35" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" t="s">
+        <v>316</v>
+      </c>
+      <c r="H36" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated reference sequences + associated data
</commit_message>
<xml_diff>
--- a/tabular/ifnl-data.xlsx
+++ b/tabular/ifnl-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="460" windowWidth="39100" windowHeight="22820" tabRatio="500"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="39120" windowHeight="22820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="A+B" sheetId="2" r:id="rId1"/>
@@ -1308,9 +1308,6 @@
     <t>IFNLA_Psi_Hsa</t>
   </si>
   <si>
-    <t>Lineage</t>
-  </si>
-  <si>
     <t>?-Rodentia</t>
   </si>
   <si>
@@ -1558,6 +1555,9 @@
   </si>
   <si>
     <t>Marsupials</t>
+  </si>
+  <si>
+    <t>Clade</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1707,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="369">
+  <cellStyleXfs count="387">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2098,7 +2116,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="369">
+  <cellStyles count="387">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2283,6 +2301,15 @@
     <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2467,6 +2494,15 @@
     <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2814,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A101" sqref="A1:A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2862,10 +2898,10 @@
         <v>382</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>429</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2879,7 +2915,7 @@
         <v>115</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>195</v>
@@ -2900,10 +2936,10 @@
         <v>215</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M2" t="s">
         <v>195</v>
@@ -2920,7 +2956,7 @@
         <v>115</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>192</v>
@@ -2941,10 +2977,10 @@
         <v>216</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M3" t="s">
         <v>192</v>
@@ -2980,13 +3016,13 @@
         <v>242</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -3021,13 +3057,13 @@
         <v>217</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3062,13 +3098,13 @@
         <v>218</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="M6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3101,13 +3137,13 @@
         <v>243</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3140,13 +3176,13 @@
         <v>244</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -3179,13 +3215,13 @@
         <v>4</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3218,13 +3254,13 @@
         <v>245</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3257,13 +3293,13 @@
         <v>246</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3298,13 +3334,13 @@
         <v>2</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3333,13 +3369,13 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -3372,13 +3408,13 @@
         <v>6</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -3411,13 +3447,13 @@
         <v>247</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -3450,13 +3486,13 @@
         <v>248</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -3489,13 +3525,13 @@
         <v>8</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -3530,13 +3566,13 @@
         <v>221</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="M18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -3571,13 +3607,13 @@
         <v>222</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -3610,13 +3646,13 @@
         <v>249</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -3649,13 +3685,13 @@
         <v>250</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -3688,13 +3724,13 @@
         <v>251</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="M22" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3727,13 +3763,13 @@
         <v>252</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -3766,13 +3802,13 @@
         <v>253</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3805,13 +3841,13 @@
         <v>254</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="M25" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -3844,13 +3880,13 @@
         <v>255</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M26" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -3879,13 +3915,13 @@
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M27" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -3918,13 +3954,13 @@
         <v>256</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="M28" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -3957,13 +3993,13 @@
         <v>257</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -3996,13 +4032,13 @@
         <v>258</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="M30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -4037,13 +4073,13 @@
         <v>223</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -4078,13 +4114,13 @@
         <v>224</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M32" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -4117,13 +4153,13 @@
         <v>260</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="M33" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -4156,13 +4192,13 @@
         <v>4</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L34" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="M34" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -4195,13 +4231,13 @@
         <v>259</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L35" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="M35" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -4234,13 +4270,13 @@
         <v>261</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M36" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -4273,13 +4309,13 @@
         <v>11</v>
       </c>
       <c r="K37" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="M37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -4314,13 +4350,13 @@
         <v>12</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -4353,13 +4389,13 @@
         <v>262</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M39" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -4392,13 +4428,13 @@
         <v>263</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M40" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -4431,13 +4467,13 @@
         <v>264</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M41" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="16" customHeight="1">
@@ -4470,13 +4506,13 @@
         <v>265</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="16" customHeight="1">
@@ -4509,13 +4545,13 @@
         <v>266</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M43" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -4548,13 +4584,13 @@
         <v>267</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="M44" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -4587,13 +4623,13 @@
         <v>268</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -4628,13 +4664,13 @@
         <v>225</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="M46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -4667,13 +4703,13 @@
         <v>269</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="M47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -4706,13 +4742,13 @@
         <v>270</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="M48" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -4745,13 +4781,13 @@
         <v>271</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="M49" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -4784,13 +4820,13 @@
         <v>272</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="M50" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -4823,13 +4859,13 @@
         <v>273</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="M51" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -4862,13 +4898,13 @@
         <v>274</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M52" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -4901,13 +4937,13 @@
         <v>275</v>
       </c>
       <c r="K53" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -4940,13 +4976,13 @@
         <v>276</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="M54" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -4981,13 +5017,13 @@
         <v>226</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M55" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -5020,13 +5056,13 @@
         <v>10</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -5059,13 +5095,13 @@
         <v>277</v>
       </c>
       <c r="K57" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L57" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M57" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -5098,13 +5134,13 @@
         <v>278</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L58" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M58" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="12" customFormat="1" ht="16">
@@ -5135,13 +5171,13 @@
       </c>
       <c r="J59" s="15"/>
       <c r="K59" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="L59" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="M59" t="s">
         <v>431</v>
-      </c>
-      <c r="L59" s="14" t="s">
-        <v>509</v>
-      </c>
-      <c r="M59" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -5174,13 +5210,13 @@
         <v>227</v>
       </c>
       <c r="K60" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L60" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="M60" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -5218,7 +5254,7 @@
         <v>425</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -5254,7 +5290,7 @@
         <v>425</v>
       </c>
       <c r="L62" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -5290,7 +5326,7 @@
         <v>425</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -5326,7 +5362,7 @@
         <v>425</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -5364,7 +5400,7 @@
         <v>425</v>
       </c>
       <c r="L65" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -5400,7 +5436,7 @@
         <v>425</v>
       </c>
       <c r="L66" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -5436,7 +5472,7 @@
         <v>425</v>
       </c>
       <c r="L67" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -5472,7 +5508,7 @@
         <v>425</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -5508,7 +5544,7 @@
         <v>425</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -5546,7 +5582,7 @@
         <v>425</v>
       </c>
       <c r="L70" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -5582,7 +5618,7 @@
         <v>425</v>
       </c>
       <c r="L71" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -5618,7 +5654,7 @@
         <v>425</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -5654,7 +5690,7 @@
         <v>425</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -5690,7 +5726,7 @@
         <v>425</v>
       </c>
       <c r="L74" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -5726,7 +5762,7 @@
         <v>425</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -5762,7 +5798,7 @@
         <v>425</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -5800,7 +5836,7 @@
         <v>425</v>
       </c>
       <c r="L77" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -5838,7 +5874,7 @@
         <v>425</v>
       </c>
       <c r="L78" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -5872,7 +5908,7 @@
         <v>425</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -5906,7 +5942,7 @@
         <v>425</v>
       </c>
       <c r="L80" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5940,7 +5976,7 @@
         <v>425</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -5974,7 +6010,7 @@
         <v>425</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -6008,7 +6044,7 @@
         <v>425</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -6042,7 +6078,7 @@
         <v>425</v>
       </c>
       <c r="L84" s="9" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -6076,7 +6112,7 @@
         <v>425</v>
       </c>
       <c r="L85" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -6110,7 +6146,7 @@
         <v>425</v>
       </c>
       <c r="L86" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -6144,7 +6180,7 @@
         <v>425</v>
       </c>
       <c r="L87" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -6178,7 +6214,7 @@
         <v>425</v>
       </c>
       <c r="L88" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -6212,7 +6248,7 @@
         <v>425</v>
       </c>
       <c r="L89" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -6246,7 +6282,7 @@
         <v>425</v>
       </c>
       <c r="L90" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -6280,7 +6316,7 @@
         <v>425</v>
       </c>
       <c r="L91" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -6314,7 +6350,7 @@
         <v>425</v>
       </c>
       <c r="L92" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -6348,7 +6384,7 @@
         <v>425</v>
       </c>
       <c r="L93" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -6382,7 +6418,7 @@
         <v>425</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -6416,7 +6452,7 @@
         <v>425</v>
       </c>
       <c r="L95" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -6450,7 +6486,7 @@
         <v>425</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -6484,7 +6520,7 @@
         <v>425</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -6518,7 +6554,7 @@
         <v>425</v>
       </c>
       <c r="L98" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -6552,7 +6588,7 @@
         <v>425</v>
       </c>
       <c r="L99" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -6586,7 +6622,7 @@
         <v>425</v>
       </c>
       <c r="L100" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -6620,7 +6656,7 @@
         <v>425</v>
       </c>
       <c r="L101" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -6652,7 +6688,7 @@
         <v>424</v>
       </c>
       <c r="L102" s="13" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>